<commit_message>
Optimize model for GitHub: 750 trees + 3000 features = 39.5MB
Performance-optimized configuration balancing accuracy with file size:
- Random Forest: 750 trees (down from 1000) with refined constraints
- TF-IDF: 3000 features with 3-grams (down from 5000 + 4-grams)
- Model size: 39.5MB (down from 111MB, fits GitHub 100MB limit)
- Validation accuracy: 83.8% (only -3% vs ultra-high performance)
- Training time: ~3 minutes (down from 5+ minutes)

Key optimizations:
- min_samples_split=3, min_samples_leaf=2 (prevents overfitting)
- min_df=2 (reduces vocabulary size)
- Maintains excellent cross-validation: 77.9% ± 15.6%

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/uploads/Brock_Team_2025.09_September.partial.xlsx
+++ b/uploads/Brock_Team_2025.09_September.partial.xlsx
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>0.4573677453521974</v>
+        <v>0.5548078018981921</v>
       </c>
     </row>
     <row r="3">
@@ -623,7 +623,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>0.4468099915767405</v>
+        <v>0.5419603047944329</v>
       </c>
     </row>
     <row r="4">
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>0.4053739567880309</v>
+        <v>0.4460162381501397</v>
       </c>
     </row>
     <row r="5">
@@ -745,11 +745,11 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Team admin</t>
+          <t>Projects</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>0.1755105404913823</v>
+        <v>0.2173498769621218</v>
       </c>
     </row>
     <row r="6">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>0.3326616401339002</v>
+        <v>0.3252196258328205</v>
       </c>
     </row>
     <row r="7">
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>0.3466081163137624</v>
+        <v>0.3397276520889215</v>
       </c>
     </row>
     <row r="8">
@@ -938,7 +938,7 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>0.5297000014699389</v>
+        <v>0.5241796117354075</v>
       </c>
     </row>
     <row r="9">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>0.4468099915767405</v>
+        <v>0.5419603047944329</v>
       </c>
     </row>
     <row r="10">
@@ -1064,7 +1064,7 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>0.4053739567880309</v>
+        <v>0.4460162381501397</v>
       </c>
     </row>
     <row r="11">
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>0.319545471456176</v>
+        <v>0.3220233051307588</v>
       </c>
     </row>
     <row r="12">
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>0.2668405685763161</v>
+        <v>0.2605045893335455</v>
       </c>
     </row>
     <row r="13">
@@ -1253,7 +1253,7 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>0.4573677453521974</v>
+        <v>0.5548078018981921</v>
       </c>
     </row>
     <row r="14">
@@ -1316,7 +1316,7 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>0.4053739567880309</v>
+        <v>0.4460162381501397</v>
       </c>
     </row>
     <row r="15">
@@ -1379,7 +1379,7 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>0.1732776721317397</v>
+        <v>0.1835962072158367</v>
       </c>
     </row>
     <row r="16">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>0.1851306392720516</v>
+        <v>0.1925593899407934</v>
       </c>
     </row>
     <row r="17">
@@ -1505,7 +1505,7 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>0.2903764258814543</v>
+        <v>0.2792634088698746</v>
       </c>
     </row>
     <row r="18">
@@ -1568,7 +1568,7 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>0.4508099915767405</v>
+        <v>0.5427565072487952</v>
       </c>
     </row>
     <row r="19">
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>0.4053739567880309</v>
+        <v>0.4460162381501397</v>
       </c>
     </row>
     <row r="20">
@@ -1694,7 +1694,7 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>0.1946577573769291</v>
+        <v>0.2100750680366164</v>
       </c>
     </row>
     <row r="21">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>0.4751860325551629</v>
+        <v>0.4539460148004327</v>
       </c>
     </row>
     <row r="22">
@@ -1820,7 +1820,7 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>0.4989550476391101</v>
+        <v>0.5180674302777326</v>
       </c>
     </row>
     <row r="23">
@@ -1883,7 +1883,7 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>0.4573677453521974</v>
+        <v>0.5548078018981921</v>
       </c>
     </row>
     <row r="24">
@@ -1946,7 +1946,7 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>0.4053739567880309</v>
+        <v>0.4460162381501397</v>
       </c>
     </row>
     <row r="25">
@@ -2009,7 +2009,7 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>0.3564271770345491</v>
+        <v>0.3411536331441269</v>
       </c>
     </row>
     <row r="26">
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>0.3417584265429391</v>
+        <v>0.3402592050763256</v>
       </c>
     </row>
     <row r="27">
@@ -2135,7 +2135,7 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>0.3636012296693453</v>
+        <v>0.3938199241899451</v>
       </c>
     </row>
     <row r="28">
@@ -2198,7 +2198,7 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>0.4064453920451315</v>
+        <v>0.4094479288197889</v>
       </c>
     </row>
     <row r="29">
@@ -2261,7 +2261,7 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>0.4573677453521974</v>
+        <v>0.5548078018981921</v>
       </c>
     </row>
     <row r="30">
@@ -2324,7 +2324,7 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>0.4053739567880309</v>
+        <v>0.4460162381501397</v>
       </c>
     </row>
     <row r="31">
@@ -2383,7 +2383,7 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>0.7080738497632085</v>
+        <v>0.7313825796431348</v>
       </c>
     </row>
     <row r="32">
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>0.7080738497632085</v>
+        <v>0.7313825796431348</v>
       </c>
     </row>
     <row r="33">
@@ -2501,7 +2501,7 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>0.7080738497632085</v>
+        <v>0.7313825796431348</v>
       </c>
     </row>
     <row r="34">
@@ -2560,7 +2560,7 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>0.7080738497632085</v>
+        <v>0.7313825796431348</v>
       </c>
     </row>
     <row r="35">
@@ -2619,7 +2619,7 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>0.7080738497632085</v>
+        <v>0.7313825796431348</v>
       </c>
     </row>
     <row r="36">
@@ -2678,7 +2678,7 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>0.3319993466624949</v>
+        <v>0.3439962146060987</v>
       </c>
     </row>
     <row r="37">
@@ -2741,7 +2741,7 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>0.3362674355253917</v>
+        <v>0.383034611212319</v>
       </c>
     </row>
     <row r="38">
@@ -2804,7 +2804,7 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>0.3547759564019523</v>
+        <v>0.4448307861986882</v>
       </c>
     </row>
     <row r="39">
@@ -2867,7 +2867,7 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>0.3426544238332555</v>
+        <v>0.4350880514236045</v>
       </c>
     </row>
     <row r="40">
@@ -2926,7 +2926,7 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>0.2609887592079594</v>
+        <v>0.3136951684244212</v>
       </c>
     </row>
     <row r="41">
@@ -2989,7 +2989,7 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>0.3445920917877729</v>
+        <v>0.4328361665953247</v>
       </c>
     </row>
     <row r="42">
@@ -3048,7 +3048,7 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>0.3123616819968877</v>
+        <v>0.3819355415348021</v>
       </c>
     </row>
     <row r="43">
@@ -3111,7 +3111,7 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>0.987097743125004</v>
+        <v>0.996354430399098</v>
       </c>
     </row>
     <row r="44">
@@ -3170,7 +3170,7 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>0.2685157460857647</v>
+        <v>0.3326751870810011</v>
       </c>
     </row>
     <row r="45">
@@ -3229,7 +3229,7 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>0.2609887592079594</v>
+        <v>0.323989365175611</v>
       </c>
     </row>
     <row r="46">
@@ -3292,7 +3292,7 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>0.7085974694915094</v>
+        <v>0.7451046325920873</v>
       </c>
     </row>
     <row r="47">
@@ -3355,7 +3355,7 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>0.3445920917877729</v>
+        <v>0.4328361665953247</v>
       </c>
     </row>
     <row r="48">
@@ -3418,7 +3418,7 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>0.387936250444444</v>
+        <v>0.409798390117203</v>
       </c>
     </row>
     <row r="49">
@@ -3481,7 +3481,7 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>0.7259834666657857</v>
+        <v>0.8091063784173107</v>
       </c>
     </row>
     <row r="50">
@@ -3544,7 +3544,7 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>0.5812661708619922</v>
+        <v>0.6664335181215053</v>
       </c>
     </row>
     <row r="51">
@@ -3607,7 +3607,7 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>0.987097743125004</v>
+        <v>0.996354430399098</v>
       </c>
     </row>
     <row r="52">
@@ -3670,7 +3670,7 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>0.510735051251484</v>
+        <v>0.5846749412904434</v>
       </c>
     </row>
     <row r="53">
@@ -3733,7 +3733,7 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>0.7202031996757102</v>
+        <v>0.7873728157726808</v>
       </c>
     </row>
     <row r="54">
@@ -3792,7 +3792,7 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>0.3205089517083323</v>
+        <v>0.3354739823213447</v>
       </c>
     </row>
     <row r="55">
@@ -3851,7 +3851,7 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>0.2909113344160474</v>
+        <v>0.2994160864186758</v>
       </c>
     </row>
     <row r="56">
@@ -3914,7 +3914,7 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>0.3185015994014496</v>
+        <v>0.3973360424669405</v>
       </c>
     </row>
     <row r="57">
@@ -3977,7 +3977,7 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>0.7259834666657857</v>
+        <v>0.8091063784173107</v>
       </c>
     </row>
     <row r="58">
@@ -4040,7 +4040,7 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>0.6423551865683725</v>
+        <v>0.5748159637577733</v>
       </c>
     </row>
     <row r="59">
@@ -4103,7 +4103,7 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>0.5891700270884929</v>
+        <v>0.6704843108961825</v>
       </c>
     </row>
     <row r="60">
@@ -4166,7 +4166,7 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>0.987097743125004</v>
+        <v>0.996354430399098</v>
       </c>
     </row>
     <row r="61">
@@ -4229,7 +4229,7 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>0.63111323916911</v>
+        <v>0.5682857256113341</v>
       </c>
     </row>
     <row r="62">
@@ -4292,7 +4292,7 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>0.5141495660029957</v>
+        <v>0.5768231781074056</v>
       </c>
     </row>
     <row r="63">
@@ -4355,7 +4355,7 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>0.7223912191842459</v>
+        <v>0.7854552496385425</v>
       </c>
     </row>
     <row r="64">
@@ -4418,7 +4418,7 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>0.3871123891493082</v>
+        <v>0.4238424624871966</v>
       </c>
     </row>
     <row r="65">
@@ -4481,7 +4481,7 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>0.3854450835075017</v>
+        <v>0.424451551797252</v>
       </c>
     </row>
     <row r="66">
@@ -4544,7 +4544,7 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>0.9909472910498738</v>
+        <v>0.996354430399098</v>
       </c>
     </row>
     <row r="67">
@@ -4607,7 +4607,7 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>0.3863101141463895</v>
+        <v>0.4253504724450449</v>
       </c>
     </row>
     <row r="68">
@@ -4666,7 +4666,7 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>0.9629701141511725</v>
+        <v>0.9673268253233595</v>
       </c>
     </row>
     <row r="69">
@@ -4729,7 +4729,7 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>0.3735832693087575</v>
+        <v>0.3948480240111621</v>
       </c>
     </row>
     <row r="70">
@@ -4792,7 +4792,7 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>0.3875463284196267</v>
+        <v>0.4238782633826745</v>
       </c>
     </row>
     <row r="71">
@@ -4855,7 +4855,7 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>0.5883364592249091</v>
+        <v>0.6670049004377965</v>
       </c>
     </row>
     <row r="72">
@@ -4918,7 +4918,7 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>0.987097743125004</v>
+        <v>0.996354430399098</v>
       </c>
     </row>
     <row r="73">
@@ -4981,7 +4981,7 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>0.3863101141463895</v>
+        <v>0.4253504724450449</v>
       </c>
     </row>
     <row r="74">
@@ -5040,7 +5040,7 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>0.3141853985108172</v>
+        <v>0.3319776628512054</v>
       </c>
     </row>
     <row r="75">
@@ -5103,7 +5103,7 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>0.3601847228148192</v>
+        <v>0.3682458246201037</v>
       </c>
     </row>
     <row r="76">
@@ -5166,7 +5166,7 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>0.3632622467960739</v>
+        <v>0.4315671964105545</v>
       </c>
     </row>
     <row r="77">
@@ -5225,11 +5225,11 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Projects</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>0.3328765460161724</v>
+        <v>0.353798639794917</v>
       </c>
     </row>
     <row r="78">
@@ -5292,7 +5292,7 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>0.3749473851109427</v>
+        <v>0.4283617722452107</v>
       </c>
     </row>
     <row r="79">
@@ -5355,7 +5355,7 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>0.588991594114174</v>
+        <v>0.6703771518057126</v>
       </c>
     </row>
     <row r="80">
@@ -5418,7 +5418,7 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>0.987097743125004</v>
+        <v>0.996354430399098</v>
       </c>
     </row>
     <row r="81">
@@ -5481,7 +5481,7 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>0.4111097859910756</v>
+        <v>0.4456396630550092</v>
       </c>
     </row>
     <row r="82">
@@ -5536,11 +5536,11 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>NSP 24-AWS DE Training Project</t>
+          <t>Holiday</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>0.222270903448796</v>
+        <v>0.241477848328965</v>
       </c>
     </row>
     <row r="83">
@@ -5599,7 +5599,7 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>0.3624771538617764</v>
+        <v>0.4530149457270521</v>
       </c>
     </row>
     <row r="84">
@@ -5662,7 +5662,7 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>0.987097743125004</v>
+        <v>0.996354430399098</v>
       </c>
     </row>
     <row r="85">
@@ -5717,11 +5717,11 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>AmaliTech Internal</t>
+          <t>Holiday</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>0.2294056490755983</v>
+        <v>0.2969291462277313</v>
       </c>
     </row>
     <row r="86">
@@ -5780,7 +5780,7 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>0.3518902508047968</v>
+        <v>0.4447143382274687</v>
       </c>
     </row>
     <row r="87">
@@ -5839,7 +5839,7 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>0.2294162489736519</v>
+        <v>0.297065618547025</v>
       </c>
     </row>
     <row r="88">
@@ -5902,7 +5902,7 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>0.7401843912770233</v>
+        <v>0.8157947917642002</v>
       </c>
     </row>
     <row r="89">
@@ -5957,11 +5957,11 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>AmaliTech Internal</t>
+          <t>Holiday</t>
         </is>
       </c>
       <c r="M89" t="n">
-        <v>0.2294056490755983</v>
+        <v>0.2969291462277313</v>
       </c>
     </row>
     <row r="90">
@@ -6024,7 +6024,7 @@
         </is>
       </c>
       <c r="M90" t="n">
-        <v>0.987097743125004</v>
+        <v>0.996354430399098</v>
       </c>
     </row>
     <row r="91">
@@ -6079,11 +6079,11 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>AmaliTech Internal</t>
+          <t>Holiday</t>
         </is>
       </c>
       <c r="M91" t="n">
-        <v>0.2294056490755983</v>
+        <v>0.2969291462277313</v>
       </c>
     </row>
     <row r="92">
@@ -6146,7 +6146,7 @@
         </is>
       </c>
       <c r="M92" t="n">
-        <v>0.5080175323622468</v>
+        <v>0.5404277937190872</v>
       </c>
     </row>
     <row r="93">
@@ -6209,7 +6209,7 @@
         </is>
       </c>
       <c r="M93" t="n">
-        <v>0.9532089373465289</v>
+        <v>0.946227692543511</v>
       </c>
     </row>
     <row r="94">
@@ -6272,7 +6272,7 @@
         </is>
       </c>
       <c r="M94" t="n">
-        <v>0.5134344809708981</v>
+        <v>0.5449323275972218</v>
       </c>
     </row>
     <row r="95">
@@ -6335,7 +6335,7 @@
         </is>
       </c>
       <c r="M95" t="n">
-        <v>0.9620497819719437</v>
+        <v>0.9605538116294022</v>
       </c>
     </row>
     <row r="96">
@@ -6398,7 +6398,7 @@
         </is>
       </c>
       <c r="M96" t="n">
-        <v>0.5100622140551415</v>
+        <v>0.5430295218320838</v>
       </c>
     </row>
     <row r="97">
@@ -6524,7 +6524,7 @@
         </is>
       </c>
       <c r="M98" t="n">
-        <v>0.3619657822292157</v>
+        <v>0.3812633257061678</v>
       </c>
     </row>
     <row r="99">
@@ -6587,7 +6587,7 @@
         </is>
       </c>
       <c r="M99" t="n">
-        <v>0.9704739815246178</v>
+        <v>0.9865791123065967</v>
       </c>
     </row>
     <row r="100">
@@ -6650,7 +6650,7 @@
         </is>
       </c>
       <c r="M100" t="n">
-        <v>0.9872061030704183</v>
+        <v>0.9942366627690113</v>
       </c>
     </row>
     <row r="101">
@@ -6713,7 +6713,7 @@
         </is>
       </c>
       <c r="M101" t="n">
-        <v>0.5095416271010724</v>
+        <v>0.5441589754011007</v>
       </c>
     </row>
     <row r="102">
@@ -6776,7 +6776,7 @@
         </is>
       </c>
       <c r="M102" t="n">
-        <v>0.9925721371472038</v>
+        <v>0.991</v>
       </c>
     </row>
     <row r="103">
@@ -6835,7 +6835,7 @@
         </is>
       </c>
       <c r="M103" t="n">
-        <v>0.3747453270693761</v>
+        <v>0.351996028075373</v>
       </c>
     </row>
     <row r="104">
@@ -6898,7 +6898,7 @@
         </is>
       </c>
       <c r="M104" t="n">
-        <v>0.5131732680886881</v>
+        <v>0.5464710092238275</v>
       </c>
     </row>
     <row r="105">
@@ -7024,7 +7024,7 @@
         </is>
       </c>
       <c r="M106" t="n">
-        <v>0.3619657822292157</v>
+        <v>0.3812633257061678</v>
       </c>
     </row>
     <row r="107">
@@ -7087,7 +7087,7 @@
         </is>
       </c>
       <c r="M107" t="n">
-        <v>0.9704739815246178</v>
+        <v>0.9865791123065967</v>
       </c>
     </row>
     <row r="108">
@@ -7150,7 +7150,7 @@
         </is>
       </c>
       <c r="M108" t="n">
-        <v>0.9872061030704183</v>
+        <v>0.9942366627690113</v>
       </c>
     </row>
     <row r="109">
@@ -7213,7 +7213,7 @@
         </is>
       </c>
       <c r="M109" t="n">
-        <v>0.5148491797293262</v>
+        <v>0.5464051161978521</v>
       </c>
     </row>
     <row r="110">
@@ -7276,7 +7276,7 @@
         </is>
       </c>
       <c r="M110" t="n">
-        <v>0.9995707781325252</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="111">
@@ -7339,7 +7339,7 @@
         </is>
       </c>
       <c r="M111" t="n">
-        <v>0.9988744218572215</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="112">
@@ -7465,7 +7465,7 @@
         </is>
       </c>
       <c r="M113" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="114">
@@ -7528,7 +7528,7 @@
         </is>
       </c>
       <c r="M114" t="n">
-        <v>0.9776177649919847</v>
+        <v>0.9894832289486538</v>
       </c>
     </row>
     <row r="115">
@@ -7591,7 +7591,7 @@
         </is>
       </c>
       <c r="M115" t="n">
-        <v>0.9872061030704183</v>
+        <v>0.9942366627690113</v>
       </c>
     </row>
     <row r="116">
@@ -7654,7 +7654,7 @@
         </is>
       </c>
       <c r="M116" t="n">
-        <v>0.5148491797293262</v>
+        <v>0.5464051161978521</v>
       </c>
     </row>
     <row r="117">
@@ -7713,7 +7713,7 @@
         </is>
       </c>
       <c r="M117" t="n">
-        <v>0.32781687322035</v>
+        <v>0.2941024604603782</v>
       </c>
     </row>
     <row r="118">
@@ -7772,7 +7772,7 @@
         </is>
       </c>
       <c r="M118" t="n">
-        <v>0.3273307409868765</v>
+        <v>0.2666407469867437</v>
       </c>
     </row>
     <row r="119">
@@ -7835,7 +7835,7 @@
         </is>
       </c>
       <c r="M119" t="n">
-        <v>0.2153048436094253</v>
+        <v>0.2175161352041525</v>
       </c>
     </row>
     <row r="120">
@@ -7961,7 +7961,7 @@
         </is>
       </c>
       <c r="M121" t="n">
-        <v>0.3619657822292157</v>
+        <v>0.3812633257061678</v>
       </c>
     </row>
     <row r="122">
@@ -8024,7 +8024,7 @@
         </is>
       </c>
       <c r="M122" t="n">
-        <v>0.9704739815246178</v>
+        <v>0.9865791123065967</v>
       </c>
     </row>
     <row r="123">
@@ -8087,7 +8087,7 @@
         </is>
       </c>
       <c r="M123" t="n">
-        <v>0.9872061030704183</v>
+        <v>0.9942366627690113</v>
       </c>
     </row>
     <row r="124">
@@ -8146,7 +8146,7 @@
         </is>
       </c>
       <c r="M124" t="n">
-        <v>0.343829336923457</v>
+        <v>0.2992289941813865</v>
       </c>
     </row>
     <row r="125">
@@ -8209,7 +8209,7 @@
         </is>
       </c>
       <c r="M125" t="n">
-        <v>0.9542912158275415</v>
+        <v>0.947227692543511</v>
       </c>
     </row>
     <row r="126">
@@ -8272,7 +8272,7 @@
         </is>
       </c>
       <c r="M126" t="n">
-        <v>0.2619826995378179</v>
+        <v>0.2607591046587717</v>
       </c>
     </row>
     <row r="127">
@@ -8398,7 +8398,7 @@
         </is>
       </c>
       <c r="M128" t="n">
-        <v>0.3563282049558886</v>
+        <v>0.3748651222485724</v>
       </c>
     </row>
     <row r="129">
@@ -8461,7 +8461,7 @@
         </is>
       </c>
       <c r="M129" t="n">
-        <v>0.9704739815246178</v>
+        <v>0.9865791123065967</v>
       </c>
     </row>
     <row r="130">
@@ -8524,7 +8524,7 @@
         </is>
       </c>
       <c r="M130" t="n">
-        <v>0.9872061030704183</v>
+        <v>0.9942366627690113</v>
       </c>
     </row>
     <row r="131">
@@ -8587,7 +8587,7 @@
         </is>
       </c>
       <c r="M131" t="n">
-        <v>0.2594138855834699</v>
+        <v>0.290266768159542</v>
       </c>
     </row>
     <row r="132">
@@ -8650,7 +8650,7 @@
         </is>
       </c>
       <c r="M132" t="n">
-        <v>0.1770272490509986</v>
+        <v>0.2101130510749856</v>
       </c>
     </row>
     <row r="133">
@@ -8713,7 +8713,7 @@
         </is>
       </c>
       <c r="M133" t="n">
-        <v>0.1832370153392555</v>
+        <v>0.210449074782104</v>
       </c>
     </row>
     <row r="134">
@@ -8776,7 +8776,7 @@
         </is>
       </c>
       <c r="M134" t="n">
-        <v>0.9702330927833305</v>
+        <v>0.986</v>
       </c>
     </row>
     <row r="135">
@@ -8839,7 +8839,7 @@
         </is>
       </c>
       <c r="M135" t="n">
-        <v>0.3126519021739435</v>
+        <v>0.2824484617619519</v>
       </c>
     </row>
     <row r="136">
@@ -8902,7 +8902,7 @@
         </is>
       </c>
       <c r="M136" t="n">
-        <v>0.98</v>
+        <v>0.9889908743633278</v>
       </c>
     </row>
     <row r="137">
@@ -8965,7 +8965,7 @@
         </is>
       </c>
       <c r="M137" t="n">
-        <v>0.3123065131587631</v>
+        <v>0.281376451871681</v>
       </c>
     </row>
     <row r="138">
@@ -9091,7 +9091,7 @@
         </is>
       </c>
       <c r="M139" t="n">
-        <v>0.3620319749737756</v>
+        <v>0.3804570088895777</v>
       </c>
     </row>
     <row r="140">
@@ -9154,7 +9154,7 @@
         </is>
       </c>
       <c r="M140" t="n">
-        <v>0.9704739815246178</v>
+        <v>0.9865791123065967</v>
       </c>
     </row>
     <row r="141">
@@ -9217,7 +9217,7 @@
         </is>
       </c>
       <c r="M141" t="n">
-        <v>0.9872061030704183</v>
+        <v>0.9942366627690113</v>
       </c>
     </row>
     <row r="142">
@@ -9280,7 +9280,7 @@
         </is>
       </c>
       <c r="M142" t="n">
-        <v>0.5546738162947459</v>
+        <v>0.5688365168323852</v>
       </c>
     </row>
     <row r="143">
@@ -9343,7 +9343,7 @@
         </is>
       </c>
       <c r="M143" t="n">
-        <v>0.9643814840157765</v>
+        <v>0.986</v>
       </c>
     </row>
     <row r="144">
@@ -9406,7 +9406,7 @@
         </is>
       </c>
       <c r="M144" t="n">
-        <v>0.3129353166415355</v>
+        <v>0.3042894702391447</v>
       </c>
     </row>
     <row r="145">
@@ -9532,7 +9532,7 @@
         </is>
       </c>
       <c r="M146" t="n">
-        <v>0.3180973816524476</v>
+        <v>0.3023073389471999</v>
       </c>
     </row>
     <row r="147">
@@ -9595,7 +9595,7 @@
         </is>
       </c>
       <c r="M147" t="n">
-        <v>0.3550651053370534</v>
+        <v>0.3786314074143874</v>
       </c>
     </row>
     <row r="148">
@@ -9658,7 +9658,7 @@
         </is>
       </c>
       <c r="M148" t="n">
-        <v>0.9704739815246178</v>
+        <v>0.9865791123065967</v>
       </c>
     </row>
     <row r="149">
@@ -9721,7 +9721,7 @@
         </is>
       </c>
       <c r="M149" t="n">
-        <v>0.9872061030704183</v>
+        <v>0.9942366627690113</v>
       </c>
     </row>
     <row r="150">
@@ -9784,7 +9784,7 @@
         </is>
       </c>
       <c r="M150" t="n">
-        <v>0.5542481357470613</v>
+        <v>0.5691207655730689</v>
       </c>
     </row>
     <row r="151">
@@ -9847,7 +9847,7 @@
         </is>
       </c>
       <c r="M151" t="n">
-        <v>0.9786837687257941</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="152">
@@ -9910,7 +9910,7 @@
         </is>
       </c>
       <c r="M152" t="n">
-        <v>0.3150421430400756</v>
+        <v>0.2934477486281386</v>
       </c>
     </row>
     <row r="153">
@@ -10036,7 +10036,7 @@
         </is>
       </c>
       <c r="M154" t="n">
-        <v>0.3155266595053963</v>
+        <v>0.2925590964573658</v>
       </c>
     </row>
     <row r="155">
@@ -10099,7 +10099,7 @@
         </is>
       </c>
       <c r="M155" t="n">
-        <v>0.9776177649919847</v>
+        <v>0.9894832289486538</v>
       </c>
     </row>
     <row r="156">
@@ -10162,7 +10162,7 @@
         </is>
       </c>
       <c r="M156" t="n">
-        <v>0.9872061030704183</v>
+        <v>0.9942366627690113</v>
       </c>
     </row>
     <row r="157">
@@ -10221,7 +10221,7 @@
         </is>
       </c>
       <c r="M157" t="n">
-        <v>0.2832995364530148</v>
+        <v>0.3078980048575732</v>
       </c>
     </row>
     <row r="158">
@@ -10284,7 +10284,7 @@
         </is>
       </c>
       <c r="M158" t="n">
-        <v>0.2587550640322847</v>
+        <v>0.2948453151095138</v>
       </c>
     </row>
     <row r="159">
@@ -10347,7 +10347,7 @@
         </is>
       </c>
       <c r="M159" t="n">
-        <v>0.2572080658937967</v>
+        <v>0.2900902881286257</v>
       </c>
     </row>
     <row r="160">
@@ -10406,7 +10406,7 @@
         </is>
       </c>
       <c r="M160" t="n">
-        <v>0.9374683736563229</v>
+        <v>0.9372118600649332</v>
       </c>
     </row>
     <row r="161">
@@ -10469,7 +10469,7 @@
         </is>
       </c>
       <c r="M161" t="n">
-        <v>0.2591976359372122</v>
+        <v>0.2891275449808154</v>
       </c>
     </row>
     <row r="162">
@@ -10528,11 +10528,11 @@
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>Holiday</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="M162" t="n">
-        <v>0.1900532654879952</v>
+        <v>0.1819453491460292</v>
       </c>
     </row>
     <row r="163">
@@ -10595,7 +10595,7 @@
         </is>
       </c>
       <c r="M163" t="n">
-        <v>0.2558026056510233</v>
+        <v>0.2885777311477893</v>
       </c>
     </row>
     <row r="164">
@@ -10658,7 +10658,7 @@
         </is>
       </c>
       <c r="M164" t="n">
-        <v>0.9560866472351111</v>
+        <v>0.971</v>
       </c>
     </row>
     <row r="165">
@@ -10721,7 +10721,7 @@
         </is>
       </c>
       <c r="M165" t="n">
-        <v>0.2710536119674481</v>
+        <v>0.273593598300533</v>
       </c>
     </row>
     <row r="166">
@@ -10784,7 +10784,7 @@
         </is>
       </c>
       <c r="M166" t="n">
-        <v>0.486470252106537</v>
+        <v>0.5978339432310091</v>
       </c>
     </row>
     <row r="167">
@@ -10847,7 +10847,7 @@
         </is>
       </c>
       <c r="M167" t="n">
-        <v>0.2572080658937967</v>
+        <v>0.2900902881286257</v>
       </c>
     </row>
     <row r="168">
@@ -10910,7 +10910,7 @@
         </is>
       </c>
       <c r="M168" t="n">
-        <v>0.6382263814946916</v>
+        <v>0.7468868377244983</v>
       </c>
     </row>
     <row r="169">
@@ -10969,11 +10969,11 @@
       </c>
       <c r="L169" t="inlineStr">
         <is>
-          <t>AmaliTech Internal</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="M169" t="n">
-        <v>0.217926920138651</v>
+        <v>0.2460565261161351</v>
       </c>
     </row>
     <row r="170">
@@ -11036,7 +11036,7 @@
         </is>
       </c>
       <c r="M170" t="n">
-        <v>0.2558026056510233</v>
+        <v>0.2885777311477893</v>
       </c>
     </row>
     <row r="171">
@@ -11099,7 +11099,7 @@
         </is>
       </c>
       <c r="M171" t="n">
-        <v>0.9560866472351111</v>
+        <v>0.971</v>
       </c>
     </row>
     <row r="172">
@@ -11162,7 +11162,7 @@
         </is>
       </c>
       <c r="M172" t="n">
-        <v>0.2710536119674481</v>
+        <v>0.273593598300533</v>
       </c>
     </row>
     <row r="173">
@@ -11225,7 +11225,7 @@
         </is>
       </c>
       <c r="M173" t="n">
-        <v>0.486470252106537</v>
+        <v>0.5978339432310091</v>
       </c>
     </row>
     <row r="174">
@@ -11288,7 +11288,7 @@
         </is>
       </c>
       <c r="M174" t="n">
-        <v>0.2572080658937967</v>
+        <v>0.2900902881286257</v>
       </c>
     </row>
     <row r="175">
@@ -11351,7 +11351,7 @@
         </is>
       </c>
       <c r="M175" t="n">
-        <v>0.6382263814946916</v>
+        <v>0.7468868377244983</v>
       </c>
     </row>
     <row r="176">
@@ -11410,11 +11410,11 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>AmaliTech Internal</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="M176" t="n">
-        <v>0.217926920138651</v>
+        <v>0.2460565261161351</v>
       </c>
     </row>
     <row r="177">
@@ -11477,7 +11477,7 @@
         </is>
       </c>
       <c r="M177" t="n">
-        <v>0.2558026056510233</v>
+        <v>0.2885777311477893</v>
       </c>
     </row>
     <row r="178">
@@ -11540,7 +11540,7 @@
         </is>
       </c>
       <c r="M178" t="n">
-        <v>0.9560866472351111</v>
+        <v>0.971</v>
       </c>
     </row>
     <row r="179">
@@ -11603,7 +11603,7 @@
         </is>
       </c>
       <c r="M179" t="n">
-        <v>0.2710536119674481</v>
+        <v>0.273593598300533</v>
       </c>
     </row>
     <row r="180">
@@ -11666,7 +11666,7 @@
         </is>
       </c>
       <c r="M180" t="n">
-        <v>0.486470252106537</v>
+        <v>0.5978339432310091</v>
       </c>
     </row>
     <row r="181">
@@ -11729,7 +11729,7 @@
         </is>
       </c>
       <c r="M181" t="n">
-        <v>0.2572080658937967</v>
+        <v>0.2900902881286257</v>
       </c>
     </row>
     <row r="182">
@@ -11792,7 +11792,7 @@
         </is>
       </c>
       <c r="M182" t="n">
-        <v>0.6382263814946916</v>
+        <v>0.7468868377244983</v>
       </c>
     </row>
     <row r="183">
@@ -11855,7 +11855,7 @@
         </is>
       </c>
       <c r="M183" t="n">
-        <v>0.2572080658937967</v>
+        <v>0.2900902881286257</v>
       </c>
     </row>
     <row r="184">
@@ -11918,7 +11918,7 @@
         </is>
       </c>
       <c r="M184" t="n">
-        <v>0.3152930381823521</v>
+        <v>0.3381655104827762</v>
       </c>
     </row>
     <row r="185">
@@ -11981,7 +11981,7 @@
         </is>
       </c>
       <c r="M185" t="n">
-        <v>0.9540866472351111</v>
+        <v>0.971</v>
       </c>
     </row>
     <row r="186">
@@ -12044,7 +12044,7 @@
         </is>
       </c>
       <c r="M186" t="n">
-        <v>0.2710536119674481</v>
+        <v>0.273593598300533</v>
       </c>
     </row>
     <row r="187">
@@ -12107,7 +12107,7 @@
         </is>
       </c>
       <c r="M187" t="n">
-        <v>0.486470252106537</v>
+        <v>0.5978339432310091</v>
       </c>
     </row>
     <row r="188">
@@ -12170,7 +12170,7 @@
         </is>
       </c>
       <c r="M188" t="n">
-        <v>0.2572080658937967</v>
+        <v>0.2900902881286257</v>
       </c>
     </row>
     <row r="189">
@@ -12233,7 +12233,7 @@
         </is>
       </c>
       <c r="M189" t="n">
-        <v>0.2558026056510233</v>
+        <v>0.2885777311477893</v>
       </c>
     </row>
     <row r="190">
@@ -12296,7 +12296,7 @@
         </is>
       </c>
       <c r="M190" t="n">
-        <v>0.6360095118763113</v>
+        <v>0.7491035268227486</v>
       </c>
     </row>
     <row r="191">
@@ -12359,7 +12359,7 @@
         </is>
       </c>
       <c r="M191" t="n">
-        <v>0.6353130336493283</v>
+        <v>0.7491035268227486</v>
       </c>
     </row>
     <row r="192">
@@ -12422,7 +12422,7 @@
         </is>
       </c>
       <c r="M192" t="n">
-        <v>0.9560866472351111</v>
+        <v>0.971</v>
       </c>
     </row>
     <row r="193">
@@ -12485,7 +12485,7 @@
         </is>
       </c>
       <c r="M193" t="n">
-        <v>0.2710536119674481</v>
+        <v>0.273593598300533</v>
       </c>
     </row>
     <row r="194">
@@ -12548,7 +12548,7 @@
         </is>
       </c>
       <c r="M194" t="n">
-        <v>0.486470252106537</v>
+        <v>0.5978339432310091</v>
       </c>
     </row>
     <row r="195">
@@ -12611,7 +12611,7 @@
         </is>
       </c>
       <c r="M195" t="n">
-        <v>0.2572080658937967</v>
+        <v>0.2900902881286257</v>
       </c>
     </row>
     <row r="196">
@@ -12674,7 +12674,7 @@
         </is>
       </c>
       <c r="M196" t="n">
-        <v>0.2134214917348283</v>
+        <v>0.2015267589412488</v>
       </c>
     </row>
     <row r="197">
@@ -12737,7 +12737,7 @@
         </is>
       </c>
       <c r="M197" t="n">
-        <v>0.2591976359372122</v>
+        <v>0.2891275449808154</v>
       </c>
     </row>
     <row r="198">
@@ -12800,7 +12800,7 @@
         </is>
       </c>
       <c r="M198" t="n">
-        <v>0.2591976359372122</v>
+        <v>0.2891275449808154</v>
       </c>
     </row>
     <row r="199">
@@ -12863,7 +12863,7 @@
         </is>
       </c>
       <c r="M199" t="n">
-        <v>0.2710536119674481</v>
+        <v>0.273593598300533</v>
       </c>
     </row>
     <row r="200">
@@ -12926,7 +12926,7 @@
         </is>
       </c>
       <c r="M200" t="n">
-        <v>0.486470252106537</v>
+        <v>0.5978339432310091</v>
       </c>
     </row>
     <row r="201">
@@ -12989,7 +12989,7 @@
         </is>
       </c>
       <c r="M201" t="n">
-        <v>0.2572080658937967</v>
+        <v>0.2900902881286257</v>
       </c>
     </row>
     <row r="202">
@@ -13052,7 +13052,7 @@
         </is>
       </c>
       <c r="M202" t="n">
-        <v>0.6547218075374149</v>
+        <v>0.7734590521591669</v>
       </c>
     </row>
     <row r="203">
@@ -13115,7 +13115,7 @@
         </is>
       </c>
       <c r="M203" t="n">
-        <v>0.6353130336493283</v>
+        <v>0.7491035268227486</v>
       </c>
     </row>
     <row r="204">
@@ -13178,7 +13178,7 @@
         </is>
       </c>
       <c r="M204" t="n">
-        <v>0.9560866472351111</v>
+        <v>0.971</v>
       </c>
     </row>
     <row r="205">
@@ -13241,7 +13241,7 @@
         </is>
       </c>
       <c r="M205" t="n">
-        <v>0.2710536119674481</v>
+        <v>0.273593598300533</v>
       </c>
     </row>
     <row r="206">
@@ -13304,7 +13304,7 @@
         </is>
       </c>
       <c r="M206" t="n">
-        <v>0.486470252106537</v>
+        <v>0.5978339432310091</v>
       </c>
     </row>
     <row r="207">
@@ -13367,7 +13367,7 @@
         </is>
       </c>
       <c r="M207" t="n">
-        <v>0.2572080658937967</v>
+        <v>0.2900902881286257</v>
       </c>
     </row>
     <row r="208">
@@ -13430,7 +13430,7 @@
         </is>
       </c>
       <c r="M208" t="n">
-        <v>0.6547218075374149</v>
+        <v>0.7734590521591669</v>
       </c>
     </row>
     <row r="209">
@@ -13489,7 +13489,7 @@
         </is>
       </c>
       <c r="M209" t="n">
-        <v>0.4581282203248565</v>
+        <v>0.4307685954391002</v>
       </c>
     </row>
     <row r="210">
@@ -13548,7 +13548,7 @@
         </is>
       </c>
       <c r="M210" t="n">
-        <v>0.9702375887514316</v>
+        <v>0.9695585485924784</v>
       </c>
     </row>
     <row r="211">
@@ -13607,7 +13607,7 @@
         </is>
       </c>
       <c r="M211" t="n">
-        <v>0.9702375887514316</v>
+        <v>0.9695585485924784</v>
       </c>
     </row>
     <row r="212">
@@ -13666,7 +13666,7 @@
         </is>
       </c>
       <c r="M212" t="n">
-        <v>0.9702375887514316</v>
+        <v>0.9695585485924784</v>
       </c>
     </row>
     <row r="213">
@@ -13725,7 +13725,7 @@
         </is>
       </c>
       <c r="M213" t="n">
-        <v>0.9702375887514316</v>
+        <v>0.9695585485924784</v>
       </c>
     </row>
     <row r="214">
@@ -13784,7 +13784,7 @@
         </is>
       </c>
       <c r="M214" t="n">
-        <v>0.9702375887514316</v>
+        <v>0.9695585485924784</v>
       </c>
     </row>
     <row r="215">
@@ -13839,11 +13839,11 @@
       </c>
       <c r="L215" t="inlineStr">
         <is>
-          <t>AmaliTech Internal</t>
+          <t>Leave</t>
         </is>
       </c>
       <c r="M215" t="n">
-        <v>0.427659422802453</v>
+        <v>0.3272469031333295</v>
       </c>
     </row>
     <row r="216">
@@ -13906,7 +13906,7 @@
         </is>
       </c>
       <c r="M216" t="n">
-        <v>0.3032683070417799</v>
+        <v>0.2981773977054531</v>
       </c>
     </row>
     <row r="217">
@@ -13961,11 +13961,11 @@
       </c>
       <c r="L217" t="inlineStr">
         <is>
-          <t>AmaliTech Internal</t>
+          <t>Leave</t>
         </is>
       </c>
       <c r="M217" t="n">
-        <v>0.427659422802453</v>
+        <v>0.3272469031333295</v>
       </c>
     </row>
     <row r="218">
@@ -14028,7 +14028,7 @@
         </is>
       </c>
       <c r="M218" t="n">
-        <v>0.2333508250867191</v>
+        <v>0.2333102521401949</v>
       </c>
     </row>
     <row r="219">
@@ -14091,7 +14091,7 @@
         </is>
       </c>
       <c r="M219" t="n">
-        <v>0.9311606224897109</v>
+        <v>0.9814554516543406</v>
       </c>
     </row>
     <row r="220">
@@ -14154,7 +14154,7 @@
         </is>
       </c>
       <c r="M220" t="n">
-        <v>0.8535903200422394</v>
+        <v>0.9215167724531967</v>
       </c>
     </row>
     <row r="221">
@@ -14217,7 +14217,7 @@
         </is>
       </c>
       <c r="M221" t="n">
-        <v>0.2333508250867191</v>
+        <v>0.2333102521401949</v>
       </c>
     </row>
     <row r="222">
@@ -14280,7 +14280,7 @@
         </is>
       </c>
       <c r="M222" t="n">
-        <v>0.3065540629600223</v>
+        <v>0.3051987262784654</v>
       </c>
     </row>
     <row r="223">
@@ -14343,7 +14343,7 @@
         </is>
       </c>
       <c r="M223" t="n">
-        <v>0.2434202868372539</v>
+        <v>0.2421317186765921</v>
       </c>
     </row>
     <row r="224">
@@ -14402,11 +14402,11 @@
       </c>
       <c r="L224" t="inlineStr">
         <is>
-          <t>Projects</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="M224" t="n">
-        <v>0.3103116385959402</v>
+        <v>0.2690045980162974</v>
       </c>
     </row>
     <row r="225">
@@ -14469,7 +14469,7 @@
         </is>
       </c>
       <c r="M225" t="n">
-        <v>0.9310210358298662</v>
+        <v>0.9805620420885734</v>
       </c>
     </row>
     <row r="226">
@@ -14532,7 +14532,7 @@
         </is>
       </c>
       <c r="M226" t="n">
-        <v>0.8535903200422394</v>
+        <v>0.9215167724531967</v>
       </c>
     </row>
     <row r="227">
@@ -14587,11 +14587,11 @@
       </c>
       <c r="L227" t="inlineStr">
         <is>
-          <t>AmaliTech Internal</t>
+          <t>Leave</t>
         </is>
       </c>
       <c r="M227" t="n">
-        <v>0.3946543581424861</v>
+        <v>0.3570655449330788</v>
       </c>
     </row>
     <row r="228">
@@ -14654,7 +14654,7 @@
         </is>
       </c>
       <c r="M228" t="n">
-        <v>0.430694605324877</v>
+        <v>0.48439465381575</v>
       </c>
     </row>
     <row r="229">
@@ -14713,7 +14713,7 @@
         </is>
       </c>
       <c r="M229" t="n">
-        <v>0.5009983394312119</v>
+        <v>0.2821139231559367</v>
       </c>
     </row>
     <row r="230">
@@ -14776,7 +14776,7 @@
         </is>
       </c>
       <c r="M230" t="n">
-        <v>0.3913452961846851</v>
+        <v>0.5006176778339518</v>
       </c>
     </row>
     <row r="231">
@@ -14835,11 +14835,11 @@
       </c>
       <c r="L231" t="inlineStr">
         <is>
-          <t>Projects</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="M231" t="n">
-        <v>0.3103116385959402</v>
+        <v>0.2690045980162974</v>
       </c>
     </row>
     <row r="232">
@@ -14902,7 +14902,7 @@
         </is>
       </c>
       <c r="M232" t="n">
-        <v>0.9310210358298662</v>
+        <v>0.9805620420885734</v>
       </c>
     </row>
     <row r="233">
@@ -14965,7 +14965,7 @@
         </is>
       </c>
       <c r="M233" t="n">
-        <v>0.8535903200422394</v>
+        <v>0.9215167724531967</v>
       </c>
     </row>
     <row r="234">
@@ -15028,7 +15028,7 @@
         </is>
       </c>
       <c r="M234" t="n">
-        <v>0.7447639231996882</v>
+        <v>0.8451559390354429</v>
       </c>
     </row>
     <row r="235">
@@ -15091,7 +15091,7 @@
         </is>
       </c>
       <c r="M235" t="n">
-        <v>0.7247859342777827</v>
+        <v>0.8210849586425871</v>
       </c>
     </row>
     <row r="236">
@@ -15154,7 +15154,7 @@
         </is>
       </c>
       <c r="M236" t="n">
-        <v>0.5094909146554707</v>
+        <v>0.6054759801523124</v>
       </c>
     </row>
     <row r="237">
@@ -15217,7 +15217,7 @@
         </is>
       </c>
       <c r="M237" t="n">
-        <v>0.4487021486934489</v>
+        <v>0.4936855351156236</v>
       </c>
     </row>
     <row r="238">
@@ -15280,7 +15280,7 @@
         </is>
       </c>
       <c r="M238" t="n">
-        <v>0.9310210358298662</v>
+        <v>0.9805620420885734</v>
       </c>
     </row>
     <row r="239">
@@ -15343,7 +15343,7 @@
         </is>
       </c>
       <c r="M239" t="n">
-        <v>0.8535903200422394</v>
+        <v>0.9215167724531967</v>
       </c>
     </row>
     <row r="240">
@@ -15406,7 +15406,7 @@
         </is>
       </c>
       <c r="M240" t="n">
-        <v>0.7447639231996882</v>
+        <v>0.8451559390354429</v>
       </c>
     </row>
     <row r="241">
@@ -15469,7 +15469,7 @@
         </is>
       </c>
       <c r="M241" t="n">
-        <v>0.728629502656986</v>
+        <v>0.8258810046451001</v>
       </c>
     </row>
     <row r="242">
@@ -15532,7 +15532,7 @@
         </is>
       </c>
       <c r="M242" t="n">
-        <v>0.4487021486934489</v>
+        <v>0.4936855351156236</v>
       </c>
     </row>
     <row r="243">
@@ -15595,7 +15595,7 @@
         </is>
       </c>
       <c r="M243" t="n">
-        <v>0.9310210358298662</v>
+        <v>0.9805620420885734</v>
       </c>
     </row>
     <row r="244">
@@ -15658,7 +15658,7 @@
         </is>
       </c>
       <c r="M244" t="n">
-        <v>0.8535903200422394</v>
+        <v>0.9215167724531967</v>
       </c>
     </row>
     <row r="245">
@@ -15717,7 +15717,7 @@
         </is>
       </c>
       <c r="M245" t="n">
-        <v>0.9061104239735294</v>
+        <v>0.904553859707786</v>
       </c>
     </row>
     <row r="246">
@@ -15776,11 +15776,11 @@
       </c>
       <c r="L246" t="inlineStr">
         <is>
-          <t>Projects</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="M246" t="n">
-        <v>0.2915898532384954</v>
+        <v>0.2918860923118817</v>
       </c>
     </row>
     <row r="247">
@@ -15843,7 +15843,7 @@
         </is>
       </c>
       <c r="M247" t="n">
-        <v>0.4487021486934489</v>
+        <v>0.4936855351156236</v>
       </c>
     </row>
     <row r="248">
@@ -15906,7 +15906,7 @@
         </is>
       </c>
       <c r="M248" t="n">
-        <v>0.9310210358298662</v>
+        <v>0.9805620420885734</v>
       </c>
     </row>
     <row r="249">
@@ -15969,7 +15969,7 @@
         </is>
       </c>
       <c r="M249" t="n">
-        <v>0.8535903200422394</v>
+        <v>0.9215167724531967</v>
       </c>
     </row>
     <row r="250">
@@ -16032,7 +16032,7 @@
         </is>
       </c>
       <c r="M250" t="n">
-        <v>0.7247859342777827</v>
+        <v>0.8210849586425871</v>
       </c>
     </row>
     <row r="251">
@@ -16095,7 +16095,7 @@
         </is>
       </c>
       <c r="M251" t="n">
-        <v>0.4419467425774021</v>
+        <v>0.4275609243326376</v>
       </c>
     </row>
     <row r="252">
@@ -16158,7 +16158,7 @@
         </is>
       </c>
       <c r="M252" t="n">
-        <v>0.4464457038525092</v>
+        <v>0.5142946963721488</v>
       </c>
     </row>
     <row r="253">
@@ -16221,7 +16221,7 @@
         </is>
       </c>
       <c r="M253" t="n">
-        <v>0.4487021486934489</v>
+        <v>0.4936855351156236</v>
       </c>
     </row>
     <row r="254">
@@ -16284,7 +16284,7 @@
         </is>
       </c>
       <c r="M254" t="n">
-        <v>0.9310210358298662</v>
+        <v>0.9805620420885734</v>
       </c>
     </row>
     <row r="255">
@@ -16347,7 +16347,7 @@
         </is>
       </c>
       <c r="M255" t="n">
-        <v>0.8535903200422394</v>
+        <v>0.9215167724531967</v>
       </c>
     </row>
     <row r="256">
@@ -16410,7 +16410,7 @@
         </is>
       </c>
       <c r="M256" t="n">
-        <v>0.727299987593274</v>
+        <v>0.8237287739100589</v>
       </c>
     </row>
     <row r="257">
@@ -16469,7 +16469,7 @@
         </is>
       </c>
       <c r="M257" t="n">
-        <v>0.4280635244150964</v>
+        <v>0.2813320132593035</v>
       </c>
     </row>
     <row r="258">
@@ -16528,7 +16528,7 @@
         </is>
       </c>
       <c r="M258" t="n">
-        <v>0.3863667136768447</v>
+        <v>0.2313401496792432</v>
       </c>
     </row>
     <row r="259">
@@ -16591,7 +16591,7 @@
         </is>
       </c>
       <c r="M259" t="n">
-        <v>0.4493451008125986</v>
+        <v>0.4895177262440688</v>
       </c>
     </row>
     <row r="260">
@@ -16654,7 +16654,7 @@
         </is>
       </c>
       <c r="M260" t="n">
-        <v>0.9310210358298662</v>
+        <v>0.9805620420885734</v>
       </c>
     </row>
     <row r="261">
@@ -16717,7 +16717,7 @@
         </is>
       </c>
       <c r="M261" t="n">
-        <v>0.8535903200422394</v>
+        <v>0.9215167724531967</v>
       </c>
     </row>
     <row r="262">
@@ -16780,7 +16780,7 @@
         </is>
       </c>
       <c r="M262" t="n">
-        <v>0.7447639231996882</v>
+        <v>0.8451559390354429</v>
       </c>
     </row>
     <row r="263">
@@ -16843,7 +16843,7 @@
         </is>
       </c>
       <c r="M263" t="n">
-        <v>0.5094909146554707</v>
+        <v>0.6054759801523124</v>
       </c>
     </row>
     <row r="264">
@@ -16902,7 +16902,7 @@
         </is>
       </c>
       <c r="M264" t="n">
-        <v>0.4079943995978653</v>
+        <v>0.2603344643549038</v>
       </c>
     </row>
     <row r="265">
@@ -16965,7 +16965,7 @@
         </is>
       </c>
       <c r="M265" t="n">
-        <v>0.4493451008125986</v>
+        <v>0.4895177262440688</v>
       </c>
     </row>
     <row r="266">
@@ -17028,7 +17028,7 @@
         </is>
       </c>
       <c r="M266" t="n">
-        <v>0.9310210358298662</v>
+        <v>0.9805620420885734</v>
       </c>
     </row>
     <row r="267">
@@ -17091,7 +17091,7 @@
         </is>
       </c>
       <c r="M267" t="n">
-        <v>0.8535903200422394</v>
+        <v>0.9215167724531967</v>
       </c>
     </row>
     <row r="268">
@@ -17150,7 +17150,7 @@
         </is>
       </c>
       <c r="M268" t="n">
-        <v>0.3081290764298127</v>
+        <v>0.3380687097127251</v>
       </c>
     </row>
     <row r="269">
@@ -17213,7 +17213,7 @@
         </is>
       </c>
       <c r="M269" t="n">
-        <v>0.4458933150710059</v>
+        <v>0.4699493324781518</v>
       </c>
     </row>
     <row r="270">
@@ -17276,7 +17276,7 @@
         </is>
       </c>
       <c r="M270" t="n">
-        <v>0.4457788604920871</v>
+        <v>0.4709420864196761</v>
       </c>
     </row>
     <row r="271">
@@ -17402,7 +17402,7 @@
         </is>
       </c>
       <c r="M272" t="n">
-        <v>0.996</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="273">
@@ -17465,7 +17465,7 @@
         </is>
       </c>
       <c r="M273" t="n">
-        <v>0.9794109742815483</v>
+        <v>0.9950145843520666</v>
       </c>
     </row>
     <row r="274">
@@ -17528,7 +17528,7 @@
         </is>
       </c>
       <c r="M274" t="n">
-        <v>0.4016291125705079</v>
+        <v>0.4257596605394668</v>
       </c>
     </row>
     <row r="275">
@@ -17591,7 +17591,7 @@
         </is>
       </c>
       <c r="M275" t="n">
-        <v>0.9794109742815483</v>
+        <v>0.9950145843520666</v>
       </c>
     </row>
     <row r="276">
@@ -17654,7 +17654,7 @@
         </is>
       </c>
       <c r="M276" t="n">
-        <v>0.2452564184533403</v>
+        <v>0.2606713948652574</v>
       </c>
     </row>
     <row r="277">
@@ -17717,7 +17717,7 @@
         </is>
       </c>
       <c r="M277" t="n">
-        <v>0.573314500708491</v>
+        <v>0.5754204855855567</v>
       </c>
     </row>
     <row r="278">
@@ -17776,11 +17776,11 @@
       </c>
       <c r="L278" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Training &amp; Learning</t>
         </is>
       </c>
       <c r="M278" t="n">
-        <v>0.2281056688548886</v>
+        <v>0.2069782264366843</v>
       </c>
     </row>
     <row r="279">
@@ -17839,7 +17839,7 @@
         </is>
       </c>
       <c r="M279" t="n">
-        <v>0.327658950757228</v>
+        <v>0.3494193705221634</v>
       </c>
     </row>
     <row r="280">
@@ -17965,7 +17965,7 @@
         </is>
       </c>
       <c r="M281" t="n">
-        <v>0.2824645057320848</v>
+        <v>0.1862631620180088</v>
       </c>
     </row>
     <row r="282">
@@ -18028,7 +18028,7 @@
         </is>
       </c>
       <c r="M282" t="n">
-        <v>0.9794109742815483</v>
+        <v>0.9950145843520666</v>
       </c>
     </row>
     <row r="283">
@@ -18091,7 +18091,7 @@
         </is>
       </c>
       <c r="M283" t="n">
-        <v>0.4016291125705079</v>
+        <v>0.4257596605394668</v>
       </c>
     </row>
     <row r="284">
@@ -18150,7 +18150,7 @@
         </is>
       </c>
       <c r="M284" t="n">
-        <v>0.327658950757228</v>
+        <v>0.3494193705221634</v>
       </c>
     </row>
     <row r="285">
@@ -18209,11 +18209,11 @@
       </c>
       <c r="L285" t="inlineStr">
         <is>
-          <t>Support</t>
+          <t>Projects</t>
         </is>
       </c>
       <c r="M285" t="n">
-        <v>0.2211478296601072</v>
+        <v>0.2562389595433602</v>
       </c>
     </row>
     <row r="286">
@@ -18276,7 +18276,7 @@
         </is>
       </c>
       <c r="M286" t="n">
-        <v>0.99</v>
+        <v>0.9929908743633278</v>
       </c>
     </row>
     <row r="287">
@@ -18339,7 +18339,7 @@
         </is>
       </c>
       <c r="M287" t="n">
-        <v>0.9509711291829979</v>
+        <v>0.8979908743633277</v>
       </c>
     </row>
     <row r="288">
@@ -18402,7 +18402,7 @@
         </is>
       </c>
       <c r="M288" t="n">
-        <v>0.9391119403402756</v>
+        <v>0.8879908743633278</v>
       </c>
     </row>
     <row r="289">
@@ -18528,7 +18528,7 @@
         </is>
       </c>
       <c r="M290" t="n">
-        <v>0.3192055828828867</v>
+        <v>0.3008918042312544</v>
       </c>
     </row>
     <row r="291">
@@ -18591,7 +18591,7 @@
         </is>
       </c>
       <c r="M291" t="n">
-        <v>0.9794109742815483</v>
+        <v>0.9950145843520666</v>
       </c>
     </row>
     <row r="292">
@@ -18654,7 +18654,7 @@
         </is>
       </c>
       <c r="M292" t="n">
-        <v>0.3727879224885545</v>
+        <v>0.3132919915437432</v>
       </c>
     </row>
     <row r="293">
@@ -18713,11 +18713,11 @@
       </c>
       <c r="L293" t="inlineStr">
         <is>
-          <t>Support</t>
+          <t>Projects</t>
         </is>
       </c>
       <c r="M293" t="n">
-        <v>0.2261717781964351</v>
+        <v>0.2559851447748265</v>
       </c>
     </row>
     <row r="294">
@@ -18780,7 +18780,7 @@
         </is>
       </c>
       <c r="M294" t="n">
-        <v>0.2224354535402422</v>
+        <v>0.2510196470986359</v>
       </c>
     </row>
     <row r="295">
@@ -18843,7 +18843,7 @@
         </is>
       </c>
       <c r="M295" t="n">
-        <v>0.974858311349958</v>
+        <v>0.981</v>
       </c>
     </row>
     <row r="296">
@@ -18906,7 +18906,7 @@
         </is>
       </c>
       <c r="M296" t="n">
-        <v>0.9579981923937103</v>
+        <v>0.9649908743633278</v>
       </c>
     </row>
     <row r="297">
@@ -18969,7 +18969,7 @@
         </is>
       </c>
       <c r="M297" t="n">
-        <v>0.9639981923937104</v>
+        <v>0.9699908743633278</v>
       </c>
     </row>
     <row r="298">
@@ -19028,7 +19028,7 @@
         </is>
       </c>
       <c r="M298" t="n">
-        <v>0.3147111323445391</v>
+        <v>0.3290203817110027</v>
       </c>
     </row>
     <row r="299">
@@ -19091,7 +19091,7 @@
         </is>
       </c>
       <c r="M299" t="n">
-        <v>0.9794109742815483</v>
+        <v>0.9950145843520666</v>
       </c>
     </row>
     <row r="300">
@@ -19154,7 +19154,7 @@
         </is>
       </c>
       <c r="M300" t="n">
-        <v>0.4016291125705079</v>
+        <v>0.4257596605394668</v>
       </c>
     </row>
     <row r="301">
@@ -19217,7 +19217,7 @@
         </is>
       </c>
       <c r="M301" t="n">
-        <v>0.5719666216171756</v>
+        <v>0.6043159698766454</v>
       </c>
     </row>
     <row r="302">
@@ -19280,7 +19280,7 @@
         </is>
       </c>
       <c r="M302" t="n">
-        <v>0.9377636001796321</v>
+        <v>0.9250094552992576</v>
       </c>
     </row>
     <row r="303">
@@ -19406,7 +19406,7 @@
         </is>
       </c>
       <c r="M304" t="n">
-        <v>0.9579967707842244</v>
+        <v>0.9389999999999999</v>
       </c>
     </row>
     <row r="305">
@@ -19469,7 +19469,7 @@
         </is>
       </c>
       <c r="M305" t="n">
-        <v>0.9794109742815483</v>
+        <v>0.9950145843520666</v>
       </c>
     </row>
     <row r="306">
@@ -19532,7 +19532,7 @@
         </is>
       </c>
       <c r="M306" t="n">
-        <v>0.4016291125705079</v>
+        <v>0.4257596605394668</v>
       </c>
     </row>
     <row r="307">
@@ -19595,7 +19595,7 @@
         </is>
       </c>
       <c r="M307" t="n">
-        <v>0.5748348787560696</v>
+        <v>0.6015261077751338</v>
       </c>
     </row>
     <row r="308">
@@ -19658,7 +19658,7 @@
         </is>
       </c>
       <c r="M308" t="n">
-        <v>0.292148490329872</v>
+        <v>0.287834755410241</v>
       </c>
     </row>
     <row r="309">
@@ -19721,7 +19721,7 @@
         </is>
       </c>
       <c r="M309" t="n">
-        <v>0.8578435828674027</v>
+        <v>0.9350000000000001</v>
       </c>
     </row>
     <row r="310">
@@ -19847,7 +19847,7 @@
         </is>
       </c>
       <c r="M311" t="n">
-        <v>0.2653328203571652</v>
+        <v>0.2372781920595617</v>
       </c>
     </row>
     <row r="312">
@@ -19910,7 +19910,7 @@
         </is>
       </c>
       <c r="M312" t="n">
-        <v>0.9794109742815483</v>
+        <v>0.9950145843520666</v>
       </c>
     </row>
     <row r="313">
@@ -19973,7 +19973,7 @@
         </is>
       </c>
       <c r="M313" t="n">
-        <v>0.4630605391402025</v>
+        <v>0.5392293632721997</v>
       </c>
     </row>
     <row r="314">
@@ -20036,7 +20036,7 @@
         </is>
       </c>
       <c r="M314" t="n">
-        <v>0.6316860677259259</v>
+        <v>0.6953200702084098</v>
       </c>
     </row>
     <row r="315">
@@ -20099,7 +20099,7 @@
         </is>
       </c>
       <c r="M315" t="n">
-        <v>0.5496707859378177</v>
+        <v>0.6100356914169488</v>
       </c>
     </row>
     <row r="316">
@@ -20162,7 +20162,7 @@
         </is>
       </c>
       <c r="M316" t="n">
-        <v>0.7317600778884519</v>
+        <v>0.7701995393846364</v>
       </c>
     </row>
     <row r="317">
@@ -20225,7 +20225,7 @@
         </is>
       </c>
       <c r="M317" t="n">
-        <v>0.4752630426811855</v>
+        <v>0.3958452534917239</v>
       </c>
     </row>
     <row r="318">
@@ -20284,7 +20284,7 @@
         </is>
       </c>
       <c r="M318" t="n">
-        <v>0.2610069087959299</v>
+        <v>0.2894412402269734</v>
       </c>
     </row>
     <row r="319">
@@ -20339,11 +20339,11 @@
       </c>
       <c r="L319" t="inlineStr">
         <is>
-          <t>Holiday</t>
+          <t>Leave</t>
         </is>
       </c>
       <c r="M319" t="n">
-        <v>0.2474250652003612</v>
+        <v>0.2512924944761724</v>
       </c>
     </row>
     <row r="320">
@@ -20406,7 +20406,7 @@
         </is>
       </c>
       <c r="M320" t="n">
-        <v>0.4752630426811855</v>
+        <v>0.3958452534917239</v>
       </c>
     </row>
     <row r="321">
@@ -20465,7 +20465,7 @@
         </is>
       </c>
       <c r="M321" t="n">
-        <v>0.24274658018012</v>
+        <v>0.2538202573433727</v>
       </c>
     </row>
     <row r="322">
@@ -20528,7 +20528,7 @@
         </is>
       </c>
       <c r="M322" t="n">
-        <v>0.6320390005133342</v>
+        <v>0.6949093568917606</v>
       </c>
     </row>
     <row r="323">
@@ -20591,7 +20591,7 @@
         </is>
       </c>
       <c r="M323" t="n">
-        <v>0.5496707859378177</v>
+        <v>0.6100356914169488</v>
       </c>
     </row>
     <row r="324">
@@ -20654,7 +20654,7 @@
         </is>
       </c>
       <c r="M324" t="n">
-        <v>0.7317600778884519</v>
+        <v>0.7701995393846364</v>
       </c>
     </row>
     <row r="325">
@@ -20713,7 +20713,7 @@
         </is>
       </c>
       <c r="M325" t="n">
-        <v>0.8836313611284849</v>
+        <v>0.883384413176365</v>
       </c>
     </row>
     <row r="326">
@@ -20772,7 +20772,7 @@
         </is>
       </c>
       <c r="M326" t="n">
-        <v>0.8836313611284849</v>
+        <v>0.883384413176365</v>
       </c>
     </row>
     <row r="327">
@@ -20831,7 +20831,7 @@
         </is>
       </c>
       <c r="M327" t="n">
-        <v>0.8836313611284849</v>
+        <v>0.883384413176365</v>
       </c>
     </row>
     <row r="328">
@@ -20890,7 +20890,7 @@
         </is>
       </c>
       <c r="M328" t="n">
-        <v>0.8836313611284849</v>
+        <v>0.883384413176365</v>
       </c>
     </row>
     <row r="329">
@@ -20945,11 +20945,11 @@
       </c>
       <c r="L329" t="inlineStr">
         <is>
-          <t>Holiday</t>
+          <t>Leave</t>
         </is>
       </c>
       <c r="M329" t="n">
-        <v>0.305754223042927</v>
+        <v>0.2925889833698408</v>
       </c>
     </row>
     <row r="330">
@@ -21012,7 +21012,7 @@
         </is>
       </c>
       <c r="M330" t="n">
-        <v>0.4752630426811855</v>
+        <v>0.3958452534917239</v>
       </c>
     </row>
     <row r="331">
@@ -21071,11 +21071,11 @@
       </c>
       <c r="L331" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Holiday</t>
         </is>
       </c>
       <c r="M331" t="n">
-        <v>0.1843619948932834</v>
+        <v>0.1846776552777755</v>
       </c>
     </row>
     <row r="332">
@@ -21138,7 +21138,7 @@
         </is>
       </c>
       <c r="M332" t="n">
-        <v>0.7348876024620691</v>
+        <v>0.7772936926199704</v>
       </c>
     </row>
     <row r="333">
@@ -21201,7 +21201,7 @@
         </is>
       </c>
       <c r="M333" t="n">
-        <v>0.1900151375185454</v>
+        <v>0.1649099127696571</v>
       </c>
     </row>
     <row r="334">
@@ -21260,11 +21260,11 @@
       </c>
       <c r="L334" t="inlineStr">
         <is>
-          <t>Projects</t>
+          <t>NSP 24-AWS DE Training Project</t>
         </is>
       </c>
       <c r="M334" t="n">
-        <v>0.2260049018927512</v>
+        <v>0.3170024551594073</v>
       </c>
     </row>
     <row r="335">
@@ -21327,7 +21327,7 @@
         </is>
       </c>
       <c r="M335" t="n">
-        <v>0.6320390005133342</v>
+        <v>0.6949093568917606</v>
       </c>
     </row>
     <row r="336">
@@ -21386,11 +21386,11 @@
       </c>
       <c r="L336" t="inlineStr">
         <is>
-          <t>Projects</t>
+          <t>NSP 24-AWS DE Training Project</t>
         </is>
       </c>
       <c r="M336" t="n">
-        <v>0.2353200480800444</v>
+        <v>0.2582449650937613</v>
       </c>
     </row>
     <row r="337">
@@ -21453,7 +21453,7 @@
         </is>
       </c>
       <c r="M337" t="n">
-        <v>0.7348876024620691</v>
+        <v>0.7772936926199704</v>
       </c>
     </row>
     <row r="338">
@@ -21512,11 +21512,11 @@
       </c>
       <c r="L338" t="inlineStr">
         <is>
-          <t>Projects</t>
+          <t>NSP 24-AWS DE Training Project</t>
         </is>
       </c>
       <c r="M338" t="n">
-        <v>0.227095166381445</v>
+        <v>0.2692756496752173</v>
       </c>
     </row>
     <row r="339">
@@ -21575,7 +21575,7 @@
         </is>
       </c>
       <c r="M339" t="n">
-        <v>0.2572957837225895</v>
+        <v>0.2539373700764835</v>
       </c>
     </row>
     <row r="340">
@@ -21701,7 +21701,7 @@
         </is>
       </c>
       <c r="M341" t="n">
-        <v>0.5602603992625429</v>
+        <v>0.6175152429037538</v>
       </c>
     </row>
     <row r="342">
@@ -21764,7 +21764,7 @@
         </is>
       </c>
       <c r="M342" t="n">
-        <v>0.9907780747003136</v>
+        <v>0.9968931579931721</v>
       </c>
     </row>
     <row r="343">
@@ -21827,7 +21827,7 @@
         </is>
       </c>
       <c r="M343" t="n">
-        <v>0.9608515553138711</v>
+        <v>0.9896291470227071</v>
       </c>
     </row>
     <row r="344">
@@ -21890,7 +21890,7 @@
         </is>
       </c>
       <c r="M344" t="n">
-        <v>0.2072207125475195</v>
+        <v>0.2260846333346436</v>
       </c>
     </row>
     <row r="345">
@@ -21953,7 +21953,7 @@
         </is>
       </c>
       <c r="M345" t="n">
-        <v>0.2461127753682903</v>
+        <v>0.2065113207579647</v>
       </c>
     </row>
     <row r="346">
@@ -22012,7 +22012,7 @@
         </is>
       </c>
       <c r="M346" t="n">
-        <v>0.2796482834892532</v>
+        <v>0.2648045102837176</v>
       </c>
     </row>
     <row r="347">
@@ -22071,7 +22071,7 @@
         </is>
       </c>
       <c r="M347" t="n">
-        <v>0.2529518252311195</v>
+        <v>0.2655344246230896</v>
       </c>
     </row>
     <row r="348">
@@ -22134,7 +22134,7 @@
         </is>
       </c>
       <c r="M348" t="n">
-        <v>0.2465600677296434</v>
+        <v>0.2107604887855749</v>
       </c>
     </row>
     <row r="349">
@@ -22197,7 +22197,7 @@
         </is>
       </c>
       <c r="M349" t="n">
-        <v>0.3932866501457448</v>
+        <v>0.4260070344609236</v>
       </c>
     </row>
     <row r="350">
@@ -22260,7 +22260,7 @@
         </is>
       </c>
       <c r="M350" t="n">
-        <v>0.5477597514710758</v>
+        <v>0.6036449897705282</v>
       </c>
     </row>
     <row r="351">
@@ -22319,11 +22319,11 @@
       </c>
       <c r="L351" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Reporting</t>
         </is>
       </c>
       <c r="M351" t="n">
-        <v>0.1676882942601612</v>
+        <v>0.2215886877774935</v>
       </c>
     </row>
     <row r="352">
@@ -22386,7 +22386,7 @@
         </is>
       </c>
       <c r="M352" t="n">
-        <v>0.9907780747003136</v>
+        <v>0.9968931579931721</v>
       </c>
     </row>
     <row r="353">
@@ -22512,7 +22512,7 @@
         </is>
       </c>
       <c r="M354" t="n">
-        <v>0.5477597514710758</v>
+        <v>0.6036449897705282</v>
       </c>
     </row>
     <row r="355">
@@ -22575,7 +22575,7 @@
         </is>
       </c>
       <c r="M355" t="n">
-        <v>0.9907780747003136</v>
+        <v>0.9968931579931721</v>
       </c>
     </row>
     <row r="356">
@@ -22634,7 +22634,7 @@
         </is>
       </c>
       <c r="M356" t="n">
-        <v>0.2662961594015884</v>
+        <v>0.2541254930154048</v>
       </c>
     </row>
     <row r="357">
@@ -22760,7 +22760,7 @@
         </is>
       </c>
       <c r="M358" t="n">
-        <v>0.5477597514710758</v>
+        <v>0.6036449897705282</v>
       </c>
     </row>
     <row r="359">
@@ -22823,7 +22823,7 @@
         </is>
       </c>
       <c r="M359" t="n">
-        <v>0.9907780747003136</v>
+        <v>0.9968931579931721</v>
       </c>
     </row>
     <row r="360">
@@ -22882,7 +22882,7 @@
         </is>
       </c>
       <c r="M360" t="n">
-        <v>0.2953167995099442</v>
+        <v>0.2753658208292642</v>
       </c>
     </row>
     <row r="361">
@@ -22941,7 +22941,7 @@
         </is>
       </c>
       <c r="M361" t="n">
-        <v>0.2953167995099442</v>
+        <v>0.2753658208292642</v>
       </c>
     </row>
     <row r="362">
@@ -23000,7 +23000,7 @@
         </is>
       </c>
       <c r="M362" t="n">
-        <v>0.2953167995099442</v>
+        <v>0.2753658208292642</v>
       </c>
     </row>
     <row r="363">
@@ -23063,7 +23063,7 @@
         </is>
       </c>
       <c r="M363" t="n">
-        <v>0.3979746467213565</v>
+        <v>0.421412678075537</v>
       </c>
     </row>
     <row r="364">
@@ -23122,7 +23122,7 @@
         </is>
       </c>
       <c r="M364" t="n">
-        <v>0.2194188378803741</v>
+        <v>0.2747686408397685</v>
       </c>
     </row>
     <row r="365">
@@ -23181,7 +23181,7 @@
         </is>
       </c>
       <c r="M365" t="n">
-        <v>0.2838753845953333</v>
+        <v>0.2655344246230896</v>
       </c>
     </row>
     <row r="366">
@@ -23307,7 +23307,7 @@
         </is>
       </c>
       <c r="M367" t="n">
-        <v>0.5477597514710758</v>
+        <v>0.6036449897705282</v>
       </c>
     </row>
     <row r="368">
@@ -23370,7 +23370,7 @@
         </is>
       </c>
       <c r="M368" t="n">
-        <v>0.9907780747003136</v>
+        <v>0.9968931579931721</v>
       </c>
     </row>
     <row r="369">
@@ -23433,7 +23433,7 @@
         </is>
       </c>
       <c r="M369" t="n">
-        <v>0.2591590728726552</v>
+        <v>0.2766750402454765</v>
       </c>
     </row>
     <row r="370">
@@ -23559,7 +23559,7 @@
         </is>
       </c>
       <c r="M371" t="n">
-        <v>0.9907780747003136</v>
+        <v>0.9968931579931721</v>
       </c>
     </row>
     <row r="372">
@@ -23622,7 +23622,7 @@
         </is>
       </c>
       <c r="M372" t="n">
-        <v>0.4582335118764261</v>
+        <v>0.4061971123967558</v>
       </c>
     </row>
     <row r="373">
@@ -23685,7 +23685,7 @@
         </is>
       </c>
       <c r="M373" t="n">
-        <v>0.2166877725823227</v>
+        <v>0.1447851658306196</v>
       </c>
     </row>
     <row r="374">
@@ -23748,7 +23748,7 @@
         </is>
       </c>
       <c r="M374" t="n">
-        <v>0.1864798715380465</v>
+        <v>0.2122846489629855</v>
       </c>
     </row>
     <row r="375">
@@ -23811,7 +23811,7 @@
         </is>
       </c>
       <c r="M375" t="n">
-        <v>0.1524245962163335</v>
+        <v>0.1440585695068748</v>
       </c>
     </row>
     <row r="376">
@@ -23874,7 +23874,7 @@
         </is>
       </c>
       <c r="M376" t="n">
-        <v>0.2034365226983757</v>
+        <v>0.2409557303425318</v>
       </c>
     </row>
     <row r="377">
@@ -23937,7 +23937,7 @@
         </is>
       </c>
       <c r="M377" t="n">
-        <v>0.9747780747003136</v>
+        <v>0.9884118582526654</v>
       </c>
     </row>
     <row r="378">
@@ -24000,7 +24000,7 @@
         </is>
       </c>
       <c r="M378" t="n">
-        <v>0.9894980690125531</v>
+        <v>0.9954645223327927</v>
       </c>
     </row>
     <row r="379">
@@ -24063,7 +24063,7 @@
         </is>
       </c>
       <c r="M379" t="n">
-        <v>0.3614808732079983</v>
+        <v>0.2279443617902974</v>
       </c>
     </row>
     <row r="380">
@@ -24126,7 +24126,7 @@
         </is>
       </c>
       <c r="M380" t="n">
-        <v>0.5120375339706317</v>
+        <v>0.5789626246986123</v>
       </c>
     </row>
     <row r="381">
@@ -24189,7 +24189,7 @@
         </is>
       </c>
       <c r="M381" t="n">
-        <v>0.31070935415176</v>
+        <v>0.2400284931902029</v>
       </c>
     </row>
     <row r="382">
@@ -24252,7 +24252,7 @@
         </is>
       </c>
       <c r="M382" t="n">
-        <v>0.9977055687864214</v>
+        <v>0.9998312617424331</v>
       </c>
     </row>
     <row r="383">
@@ -24311,11 +24311,11 @@
       </c>
       <c r="L383" t="inlineStr">
         <is>
-          <t>Team admin</t>
+          <t>Reporting</t>
         </is>
       </c>
       <c r="M383" t="n">
-        <v>0.2460805169055633</v>
+        <v>0.2457119155006381</v>
       </c>
     </row>
     <row r="384">
@@ -24378,7 +24378,7 @@
         </is>
       </c>
       <c r="M384" t="n">
-        <v>0.3619093085278938</v>
+        <v>0.4123185009958084</v>
       </c>
     </row>
     <row r="385">
@@ -24504,7 +24504,7 @@
         </is>
       </c>
       <c r="M386" t="n">
-        <v>0.4346198690441026</v>
+        <v>0.4337350005060502</v>
       </c>
     </row>
     <row r="387">
@@ -24567,7 +24567,7 @@
         </is>
       </c>
       <c r="M387" t="n">
-        <v>0.9932452043681933</v>
+        <v>0.9959757169652483</v>
       </c>
     </row>
     <row r="388">
@@ -24630,7 +24630,7 @@
         </is>
       </c>
       <c r="M388" t="n">
-        <v>0.9977055687864214</v>
+        <v>0.9998312617424331</v>
       </c>
     </row>
     <row r="389">
@@ -24693,7 +24693,7 @@
         </is>
       </c>
       <c r="M389" t="n">
-        <v>0.3030184077045676</v>
+        <v>0.3546602877117339</v>
       </c>
     </row>
     <row r="390">
@@ -24756,7 +24756,7 @@
         </is>
       </c>
       <c r="M390" t="n">
-        <v>0.6134962824925952</v>
+        <v>0.9749792960662526</v>
       </c>
     </row>
     <row r="391">
@@ -24819,7 +24819,7 @@
         </is>
       </c>
       <c r="M391" t="n">
-        <v>0.9584363901871576</v>
+        <v>0.9709792960662526</v>
       </c>
     </row>
     <row r="392">
@@ -24882,7 +24882,7 @@
         </is>
       </c>
       <c r="M392" t="n">
-        <v>0.3030184077045676</v>
+        <v>0.3546602877117339</v>
       </c>
     </row>
     <row r="393">
@@ -25008,7 +25008,7 @@
         </is>
       </c>
       <c r="M394" t="n">
-        <v>0.428894522891703</v>
+        <v>0.423785548882663</v>
       </c>
     </row>
     <row r="395">
@@ -25071,7 +25071,7 @@
         </is>
       </c>
       <c r="M395" t="n">
-        <v>0.9932452043681933</v>
+        <v>0.9959757169652483</v>
       </c>
     </row>
     <row r="396">
@@ -25134,7 +25134,7 @@
         </is>
       </c>
       <c r="M396" t="n">
-        <v>0.9977055687864214</v>
+        <v>0.9998312617424331</v>
       </c>
     </row>
     <row r="397">
@@ -25197,7 +25197,7 @@
         </is>
       </c>
       <c r="M397" t="n">
-        <v>0.9837975824545993</v>
+        <v>0.993202530388395</v>
       </c>
     </row>
     <row r="398">
@@ -25260,7 +25260,7 @@
         </is>
       </c>
       <c r="M398" t="n">
-        <v>0.5028692114963561</v>
+        <v>0.5880427724607347</v>
       </c>
     </row>
     <row r="399">
@@ -25323,7 +25323,7 @@
         </is>
       </c>
       <c r="M399" t="n">
-        <v>0.4360054113883759</v>
+        <v>0.3862203125128462</v>
       </c>
     </row>
     <row r="400">
@@ -25449,7 +25449,7 @@
         </is>
       </c>
       <c r="M401" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.959</v>
       </c>
     </row>
     <row r="402">
@@ -25575,7 +25575,7 @@
         </is>
       </c>
       <c r="M403" t="n">
-        <v>0.497332506366248</v>
+        <v>0.5108770179582606</v>
       </c>
     </row>
     <row r="404">
@@ -25638,7 +25638,7 @@
         </is>
       </c>
       <c r="M404" t="n">
-        <v>0.428894522891703</v>
+        <v>0.423785548882663</v>
       </c>
     </row>
     <row r="405">
@@ -25701,7 +25701,7 @@
         </is>
       </c>
       <c r="M405" t="n">
-        <v>0.9932452043681933</v>
+        <v>0.9959757169652483</v>
       </c>
     </row>
     <row r="406">
@@ -25886,11 +25886,11 @@
       </c>
       <c r="L408" t="inlineStr">
         <is>
-          <t>Holiday</t>
+          <t>Leave</t>
         </is>
       </c>
       <c r="M408" t="n">
-        <v>0.2149939098031054</v>
+        <v>0.2682196050852002</v>
       </c>
     </row>
     <row r="409">
@@ -25953,7 +25953,7 @@
         </is>
       </c>
       <c r="M409" t="n">
-        <v>0.8409415776271412</v>
+        <v>0.7865295501772399</v>
       </c>
     </row>
     <row r="410">
@@ -26079,7 +26079,7 @@
         </is>
       </c>
       <c r="M411" t="n">
-        <v>0.9947882123531855</v>
+        <v>0.9976958813604353</v>
       </c>
     </row>
     <row r="412">
@@ -26142,7 +26142,7 @@
         </is>
       </c>
       <c r="M412" t="n">
-        <v>0.5618792793138884</v>
+        <v>0.6111876226073916</v>
       </c>
     </row>
     <row r="413">
@@ -26201,11 +26201,11 @@
       </c>
       <c r="L413" t="inlineStr">
         <is>
-          <t>Support</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="M413" t="n">
-        <v>0.1769876396421641</v>
+        <v>0.1992036356890338</v>
       </c>
     </row>
     <row r="414">
@@ -26268,7 +26268,7 @@
         </is>
       </c>
       <c r="M414" t="n">
-        <v>0.2808453736525818</v>
+        <v>0.3062931418043473</v>
       </c>
     </row>
     <row r="415">
@@ -26394,7 +26394,7 @@
         </is>
       </c>
       <c r="M416" t="n">
-        <v>0.9977055687864214</v>
+        <v>0.9998312617424331</v>
       </c>
     </row>
     <row r="417">
@@ -26457,7 +26457,7 @@
         </is>
       </c>
       <c r="M417" t="n">
-        <v>0.9947882123531855</v>
+        <v>0.996741123932648</v>
       </c>
     </row>
     <row r="418">
@@ -26520,7 +26520,7 @@
         </is>
       </c>
       <c r="M418" t="n">
-        <v>0.5241444120223561</v>
+        <v>0.5909511458300934</v>
       </c>
     </row>
     <row r="419">
@@ -26583,7 +26583,7 @@
         </is>
       </c>
       <c r="M419" t="n">
-        <v>0.9837975824545993</v>
+        <v>0.993202530388395</v>
       </c>
     </row>
     <row r="420">
@@ -26646,7 +26646,7 @@
         </is>
       </c>
       <c r="M420" t="n">
-        <v>0.9977055687864214</v>
+        <v>0.9998312617424331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>